<commit_message>
Include descriptions in output
</commit_message>
<xml_diff>
--- a/Loco.xlsx
+++ b/Loco.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swhitehead/NetBeansProjects/Loco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B769083-280B-694E-B1FD-22DB6330AF9D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313F7EF5-A35D-E148-9ECE-3ED1CE0C0AAD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="8460" windowWidth="38400" windowHeight="23540" xr2:uid="{1041F770-18E8-8547-86F0-5B65CA8E4B6D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Description</t>
   </si>
@@ -85,6 +85,21 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>The "hint" text used when prompting for the uer's login name</t>
+  </si>
+  <si>
+    <t>"Ok" text displayed on dialog buttons</t>
+  </si>
+  <si>
+    <t>"Cancel" text displayed on dialog buttons</t>
+  </si>
+  <si>
+    <t>"Yes" text displayed on dialog buttons when making a request from the user</t>
+  </si>
+  <si>
+    <t>"No" text displayed on dialog buttons when making a request from the user</t>
   </si>
 </sst>
 </file>
@@ -439,11 +454,12 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="43.83203125" customWidth="1"/>
     <col min="3" max="4" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -465,6 +481,9 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -476,6 +495,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -487,6 +509,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -498,6 +523,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -509,6 +537,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>

</xml_diff>